<commit_message>
Task for sprint 3
</commit_message>
<xml_diff>
--- a/Document/SCRUM/Sprint Backlog.xlsx
+++ b/Document/SCRUM/Sprint Backlog.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 2" sheetId="5" r:id="rId2"/>
-    <sheet name="Information" sheetId="4" r:id="rId3"/>
+    <sheet name="Sprint 3" sheetId="6" r:id="rId3"/>
+    <sheet name="Information" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Status">Information!$A$15:$A$19</definedName>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="78">
   <si>
     <t>No.</t>
   </si>
@@ -367,12 +368,45 @@
   <si>
     <t>HTML + CSS</t>
   </si>
+  <si>
+    <t>Implement basic function for mockups</t>
+  </si>
+  <si>
+    <t>Finish report 2</t>
+  </si>
+  <si>
+    <t>Finish custom form for medical profile</t>
+  </si>
+  <si>
+    <t>Use case description</t>
+  </si>
+  <si>
+    <t>Class diagram</t>
+  </si>
+  <si>
+    <t>Fix ERD Diagram</t>
+  </si>
+  <si>
+    <t>Fix Physical Database Diagram</t>
+  </si>
+  <si>
+    <t>Update Usecase Diagram</t>
+  </si>
+  <si>
+    <t>Use case for Patient</t>
+  </si>
+  <si>
+    <t>Usecase for Doctor</t>
+  </si>
+  <si>
+    <t>Usecase for Admin/Authorized User/Guest</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -417,6 +451,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -438,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -457,27 +497,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -511,18 +563,38 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -535,7 +607,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H14" totalsRowCount="1" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H14" totalsRowCount="1" headerRowDxfId="8">
   <autoFilter ref="A2:H13"/>
   <tableColumns count="8">
     <tableColumn id="1" name="No."/>
@@ -554,7 +626,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A2:H15" totalsRowCount="1" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A2:H15" totalsRowCount="1" headerRowDxfId="6">
   <autoFilter ref="A2:H14"/>
   <tableColumns count="8">
     <tableColumn id="1" name="No."/>
@@ -573,6 +645,25 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="A2:H15" totalsRowCount="1" headerRowDxfId="7">
+  <autoFilter ref="A2:H14"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="No."/>
+    <tableColumn id="3" name="Userstory"/>
+    <tableColumn id="7" name="Task"/>
+    <tableColumn id="4" name="Description"/>
+    <tableColumn id="8" name="Acceptance criteria"/>
+    <tableColumn id="2" name="Assign"/>
+    <tableColumn id="5" name="Estimate" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table145[Estimate])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Status"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A6:C10" totalsRowShown="0">
   <autoFilter ref="A6:C10"/>
   <tableColumns count="3">
@@ -1237,8 +1328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1300,6 +1391,9 @@
       <c r="C3" t="s">
         <v>60</v>
       </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
       <c r="G3">
         <v>2</v>
       </c>
@@ -1315,6 +1409,9 @@
         <v>61</v>
       </c>
       <c r="E4" s="2"/>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
       <c r="G4">
         <v>2</v>
       </c>
@@ -1330,6 +1427,9 @@
         <v>66</v>
       </c>
       <c r="E5" s="2"/>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1340,6 +1440,9 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1350,6 +1453,9 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1412,10 +1518,10 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H14">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Accept"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1455,6 +1561,236 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" customWidth="1"/>
+    <col min="4" max="4" width="47.42578125" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <f>SUM(Table145[Estimate])</f>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="H3:H14">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Accept"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F14">
+    <cfRule type="iconSet" priority="3">
+      <iconSet>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="#REF!"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H14">
+      <formula1>Status</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Information!$B$7:$B$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>F3:F14</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Add task for sprint 4
</commit_message>
<xml_diff>
--- a/Document/SCRUM/Sprint Backlog.xlsx
+++ b/Document/SCRUM/Sprint Backlog.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="10680" windowHeight="4650" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 2" sheetId="5" r:id="rId2"/>
     <sheet name="Sprint 3" sheetId="6" r:id="rId3"/>
-    <sheet name="Information" sheetId="4" r:id="rId4"/>
+    <sheet name="Sprint 4" sheetId="7" r:id="rId4"/>
+    <sheet name="Information" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Status">Information!$A$15:$A$19</definedName>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="89">
   <si>
     <t>No.</t>
   </si>
@@ -398,6 +399,42 @@
   <si>
     <t>Usecase for Admin/Authorized User/Guest</t>
   </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>Manage Doctor</t>
+  </si>
+  <si>
+    <t>Sequence diagram</t>
+  </si>
+  <si>
+    <t>Component Diagram</t>
+  </si>
+  <si>
+    <t>System architecture</t>
+  </si>
+  <si>
+    <t>Manage user</t>
+  </si>
+  <si>
+    <t>Manage doctor</t>
+  </si>
+  <si>
+    <t>Create, Edit, Deactive User, Assign Role for User</t>
+  </si>
+  <si>
+    <t>Add, Edit, Deactive Doctor</t>
+  </si>
+  <si>
+    <t>Manage SpecialtyField</t>
+  </si>
+  <si>
+    <t>Add Specialty, Assign SpecialtyField for Doctor</t>
+  </si>
+  <si>
+    <t>Class diagram Business Logic, Controller</t>
+  </si>
 </sst>
 </file>
 
@@ -475,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -486,6 +523,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -499,34 +539,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="13">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -560,21 +602,18 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -593,6 +632,51 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -604,7 +688,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H14" totalsRowCount="1" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H14" totalsRowCount="1" headerRowDxfId="10">
   <autoFilter ref="A2:H13"/>
   <tableColumns count="8">
     <tableColumn id="1" name="No."/>
@@ -642,8 +726,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="A2:H15" totalsRowCount="1" headerRowDxfId="6">
-  <autoFilter ref="A2:H14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="A2:H16" totalsRowCount="1" headerRowDxfId="4">
+  <autoFilter ref="A2:H15"/>
   <tableColumns count="8">
     <tableColumn id="1" name="No."/>
     <tableColumn id="3" name="Userstory"/>
@@ -661,6 +745,25 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table1456" displayName="Table1456" ref="A2:H15" totalsRowCount="1" headerRowDxfId="1">
+  <autoFilter ref="A2:H14"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="No."/>
+    <tableColumn id="3" name="Userstory"/>
+    <tableColumn id="7" name="Task"/>
+    <tableColumn id="4" name="Description" dataDxfId="0"/>
+    <tableColumn id="8" name="Acceptance criteria"/>
+    <tableColumn id="2" name="Assign"/>
+    <tableColumn id="5" name="Estimate" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table1456[Estimate])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Status"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A6:C10" totalsRowShown="0">
   <autoFilter ref="A6:C10"/>
   <tableColumns count="3">
@@ -978,15 +1081,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
       <c r="H1" s="2" t="s">
         <v>58</v>
       </c>
@@ -1289,10 +1392,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H13">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"Accept"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1342,15 +1445,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
       <c r="H1" s="2" t="s">
         <v>58</v>
       </c>
@@ -1515,10 +1618,10 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H14">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"Accept"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1558,10 +1661,279 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" customWidth="1"/>
+    <col min="4" max="4" width="47.42578125" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="2"/>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="2"/>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="2"/>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <f>SUM(Table145[Estimate])</f>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="H3:H15">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+      <formula>"Accept"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F15">
+    <cfRule type="iconSet" priority="3">
+      <iconSet>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="#REF!"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H15">
+      <formula1>Status</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Information!$B$7:$B$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>F3:F15</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1577,15 +1949,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
       <c r="H1" s="2" t="s">
         <v>58</v>
       </c>
@@ -1621,8 +1993,9 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="D3" s="5"/>
       <c r="G3">
         <v>2</v>
       </c>
@@ -1632,9 +2005,9 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="D4" s="6"/>
       <c r="E4" s="2"/>
       <c r="G4">
         <v>2</v>
@@ -1645,9 +2018,9 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="2"/>
+        <v>88</v>
+      </c>
+      <c r="D5" s="6"/>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1655,9 +2028,9 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" s="2"/>
+        <v>79</v>
+      </c>
+      <c r="D6" s="6"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1665,9 +2038,11 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" s="2"/>
+        <v>82</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>84</v>
+      </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1675,9 +2050,11 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="4"/>
+        <v>83</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1685,55 +2062,52 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="4"/>
+        <v>86</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>87</v>
+      </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="C10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
-        <v>69</v>
-      </c>
+      <c r="D11" s="5"/>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>70</v>
-      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="6"/>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
+      <c r="D14" s="5"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G15">
-        <f>SUM(Table145[Estimate])</f>
+        <f>SUM(Table1456[Estimate])</f>
         <v>4</v>
       </c>
     </row>
@@ -1742,10 +2116,10 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H14">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Accept"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1783,7 +2157,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:I19"/>
   <sheetViews>
@@ -1801,11 +2175,11 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
       <c r="H5" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Break task for Sequence diagram
</commit_message>
<xml_diff>
--- a/Document/SCRUM/Sprint Backlog.xlsx
+++ b/Document/SCRUM/Sprint Backlog.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="90">
   <si>
     <t>No.</t>
   </si>
@@ -434,6 +434,12 @@
   </si>
   <si>
     <t>Class diagram Business Logic, Controller</t>
+  </si>
+  <si>
+    <t>Define new medical profile template
+Update medical profile for patient
+View medical profile
+Request an online medical treatment</t>
   </si>
 </sst>
 </file>
@@ -1933,7 +1939,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2023,14 +2029,16 @@
       <c r="D5" s="6"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="6" t="s">
+        <v>89</v>
+      </c>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add more task for Sprint 5
</commit_message>
<xml_diff>
--- a/Document/SCRUM/Sprint Backlog.xlsx
+++ b/Document/SCRUM/Sprint Backlog.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="10680" windowHeight="4650" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="10680" windowHeight="4650" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 2" sheetId="5" r:id="rId2"/>
     <sheet name="Sprint 3" sheetId="6" r:id="rId3"/>
     <sheet name="Sprint 4" sheetId="7" r:id="rId4"/>
-    <sheet name="Information" sheetId="4" r:id="rId5"/>
+    <sheet name="Sprint 5" sheetId="8" r:id="rId5"/>
+    <sheet name="Information" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="Status">Information!$A$15:$A$19</definedName>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="98">
   <si>
     <t>No.</t>
   </si>
@@ -441,6 +442,43 @@
 View medical profile
 Request an online medical treatment
 Update Personal Health Record</t>
+  </si>
+  <si>
+    <t>Create patient style</t>
+  </si>
+  <si>
+    <t>Patient update Personal Health Record</t>
+  </si>
+  <si>
+    <t>Layout Homepage</t>
+  </si>
+  <si>
+    <t>Chatting</t>
+  </si>
+  <si>
+    <t>New medical profile template</t>
+  </si>
+  <si>
+    <t>Update system architecture</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sprint 5
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Kanban: https://trello.com/b/JditEulN/kanban-sprint-1</t>
+    </r>
+  </si>
+  <si>
+    <t>Class diagram Model</t>
   </si>
 </sst>
 </file>
@@ -546,7 +584,51 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -695,7 +777,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H14" totalsRowCount="1" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H14" totalsRowCount="1" headerRowDxfId="14">
   <autoFilter ref="A2:H13"/>
   <tableColumns count="8">
     <tableColumn id="1" name="No."/>
@@ -714,7 +796,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A2:H15" totalsRowCount="1" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A2:H15" totalsRowCount="1" headerRowDxfId="11">
   <autoFilter ref="A2:H14"/>
   <tableColumns count="8">
     <tableColumn id="1" name="No."/>
@@ -733,7 +815,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="A2:H16" totalsRowCount="1" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="A2:H16" totalsRowCount="1" headerRowDxfId="8">
   <autoFilter ref="A2:H15"/>
   <tableColumns count="8">
     <tableColumn id="1" name="No."/>
@@ -752,13 +834,13 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table1456" displayName="Table1456" ref="A2:H15" totalsRowCount="1" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table1456" displayName="Table1456" ref="A2:H15" totalsRowCount="1" headerRowDxfId="5">
   <autoFilter ref="A2:H14"/>
   <tableColumns count="8">
     <tableColumn id="1" name="No."/>
     <tableColumn id="3" name="Userstory"/>
     <tableColumn id="7" name="Task"/>
-    <tableColumn id="4" name="Description" dataDxfId="0"/>
+    <tableColumn id="4" name="Description" dataDxfId="4"/>
     <tableColumn id="8" name="Acceptance criteria"/>
     <tableColumn id="2" name="Assign"/>
     <tableColumn id="5" name="Estimate" totalsRowFunction="custom">
@@ -771,6 +853,25 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table14567" displayName="Table14567" ref="A2:H15" totalsRowCount="1" headerRowDxfId="1">
+  <autoFilter ref="A2:H14"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="No."/>
+    <tableColumn id="3" name="Userstory"/>
+    <tableColumn id="7" name="Task"/>
+    <tableColumn id="4" name="Description" dataDxfId="0"/>
+    <tableColumn id="8" name="Acceptance criteria"/>
+    <tableColumn id="2" name="Assign"/>
+    <tableColumn id="5" name="Estimate" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table14567[Estimate])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Status"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A6:C10" totalsRowShown="0">
   <autoFilter ref="A6:C10"/>
   <tableColumns count="3">
@@ -1399,10 +1500,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H13">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
       <formula>"Accept"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1435,8 +1536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,6 +1605,9 @@
       <c r="G3">
         <v>2</v>
       </c>
+      <c r="H3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1522,6 +1626,9 @@
       <c r="G4">
         <v>2</v>
       </c>
+      <c r="H4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1536,6 +1643,9 @@
       <c r="E5" s="2"/>
       <c r="F5" t="s">
         <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1549,6 +1659,9 @@
       <c r="E6" s="2"/>
       <c r="F6" t="s">
         <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1625,10 +1738,10 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H14">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"Accept"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1670,8 +1783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1739,6 +1852,9 @@
       <c r="G3">
         <v>2</v>
       </c>
+      <c r="H3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1755,6 +1871,9 @@
       <c r="G4">
         <v>2</v>
       </c>
+      <c r="H4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1768,6 +1887,9 @@
       <c r="F5" t="s">
         <v>13</v>
       </c>
+      <c r="H5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1781,6 +1903,9 @@
       <c r="F6" t="s">
         <v>17</v>
       </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1794,6 +1919,9 @@
       <c r="F7" t="s">
         <v>16</v>
       </c>
+      <c r="H7" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1807,6 +1935,9 @@
       <c r="F8" t="s">
         <v>18</v>
       </c>
+      <c r="H8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -1820,6 +1951,9 @@
       <c r="F9" t="s">
         <v>13</v>
       </c>
+      <c r="H9" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1845,6 +1979,9 @@
       <c r="F11" t="s">
         <v>17</v>
       </c>
+      <c r="H11" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1857,6 +1994,9 @@
       <c r="F12" t="s">
         <v>13</v>
       </c>
+      <c r="H12" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1868,6 +2008,9 @@
       <c r="E13" s="2"/>
       <c r="F13" t="s">
         <v>16</v>
+      </c>
+      <c r="H13" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1894,10 +2037,10 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H15">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"Accept"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1939,8 +2082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2006,6 +2149,9 @@
       <c r="G3">
         <v>2</v>
       </c>
+      <c r="H3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -2019,16 +2165,22 @@
       <c r="G4">
         <v>2</v>
       </c>
+      <c r="H4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="2"/>
+      <c r="H5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -2041,6 +2193,9 @@
         <v>89</v>
       </c>
       <c r="E6" s="2"/>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -2053,6 +2208,9 @@
         <v>84</v>
       </c>
       <c r="E7" s="2"/>
+      <c r="H7" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -2077,13 +2235,22 @@
         <v>87</v>
       </c>
       <c r="E9" s="2"/>
+      <c r="H9" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
+      <c r="C10" t="s">
+        <v>90</v>
+      </c>
       <c r="D10" s="6"/>
       <c r="E10" s="2"/>
+      <c r="H10" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -2117,6 +2284,231 @@
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G15">
         <f>SUM(Table1456[Estimate])</f>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="H3:H14">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+      <formula>"Accept"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F14">
+    <cfRule type="iconSet" priority="3">
+      <iconSet>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="#REF!"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H14">
+      <formula1>Status</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Information!$B$7:$B$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>F3:F14</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" customWidth="1"/>
+    <col min="4" max="4" width="47.42578125" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="2"/>
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <f>SUM(Table14567[Estimate])</f>
         <v>4</v>
       </c>
     </row>
@@ -2166,7 +2558,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:I19"/>
   <sheetViews>

</xml_diff>

<commit_message>
Add task for sprint 6
</commit_message>
<xml_diff>
--- a/Document/SCRUM/Sprint Backlog.xlsx
+++ b/Document/SCRUM/Sprint Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="10680" windowHeight="4650" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="10680" windowHeight="4650" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,8 @@
     <sheet name="Sprint 3" sheetId="6" r:id="rId3"/>
     <sheet name="Sprint 4" sheetId="7" r:id="rId4"/>
     <sheet name="Sprint 5" sheetId="8" r:id="rId5"/>
-    <sheet name="Information" sheetId="4" r:id="rId6"/>
+    <sheet name="Sprint 6" sheetId="9" r:id="rId6"/>
+    <sheet name="Information" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="Status">Information!$A$15:$A$19</definedName>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="104">
   <si>
     <t>No.</t>
   </si>
@@ -479,6 +480,37 @@
   </si>
   <si>
     <t>Class diagram Model</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sprint 6
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Kanban: https://trello.com/b/JditEulN/kanban-sprint-1</t>
+    </r>
+  </si>
+  <si>
+    <t>Finish Chatting</t>
+  </si>
+  <si>
+    <t>Doctor create medical profile for patient</t>
+  </si>
+  <si>
+    <t>Let user show webcam on conversation</t>
+  </si>
+  <si>
+    <t>Show Conversation List for Patient</t>
+  </si>
+  <si>
+    <t>Manage FilmType</t>
   </si>
 </sst>
 </file>
@@ -584,7 +616,51 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -777,7 +853,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H14" totalsRowCount="1" headerRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H14" totalsRowCount="1" headerRowDxfId="18">
   <autoFilter ref="A2:H13"/>
   <tableColumns count="8">
     <tableColumn id="1" name="No."/>
@@ -796,7 +872,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A2:H15" totalsRowCount="1" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A2:H15" totalsRowCount="1" headerRowDxfId="15">
   <autoFilter ref="A2:H14"/>
   <tableColumns count="8">
     <tableColumn id="1" name="No."/>
@@ -815,7 +891,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="A2:H16" totalsRowCount="1" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="A2:H16" totalsRowCount="1" headerRowDxfId="12">
   <autoFilter ref="A2:H15"/>
   <tableColumns count="8">
     <tableColumn id="1" name="No."/>
@@ -834,13 +910,13 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table1456" displayName="Table1456" ref="A2:H15" totalsRowCount="1" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table1456" displayName="Table1456" ref="A2:H15" totalsRowCount="1" headerRowDxfId="9">
   <autoFilter ref="A2:H14"/>
   <tableColumns count="8">
     <tableColumn id="1" name="No."/>
     <tableColumn id="3" name="Userstory"/>
     <tableColumn id="7" name="Task"/>
-    <tableColumn id="4" name="Description" dataDxfId="4"/>
+    <tableColumn id="4" name="Description" dataDxfId="8"/>
     <tableColumn id="8" name="Acceptance criteria"/>
     <tableColumn id="2" name="Assign"/>
     <tableColumn id="5" name="Estimate" totalsRowFunction="custom">
@@ -853,13 +929,13 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table14567" displayName="Table14567" ref="A2:H15" totalsRowCount="1" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table14567" displayName="Table14567" ref="A2:H15" totalsRowCount="1" headerRowDxfId="5">
   <autoFilter ref="A2:H14"/>
   <tableColumns count="8">
     <tableColumn id="1" name="No."/>
     <tableColumn id="3" name="Userstory"/>
     <tableColumn id="7" name="Task"/>
-    <tableColumn id="4" name="Description" dataDxfId="0"/>
+    <tableColumn id="4" name="Description" dataDxfId="4"/>
     <tableColumn id="8" name="Acceptance criteria"/>
     <tableColumn id="2" name="Assign"/>
     <tableColumn id="5" name="Estimate" totalsRowFunction="custom">
@@ -872,6 +948,25 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table145678" displayName="Table145678" ref="A2:H15" totalsRowCount="1" headerRowDxfId="1">
+  <autoFilter ref="A2:H14"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="No."/>
+    <tableColumn id="3" name="Userstory"/>
+    <tableColumn id="7" name="Task"/>
+    <tableColumn id="4" name="Description" dataDxfId="0"/>
+    <tableColumn id="8" name="Acceptance criteria"/>
+    <tableColumn id="2" name="Assign"/>
+    <tableColumn id="5" name="Estimate" totalsRowFunction="custom">
+      <totalsRowFormula>SUM(Table145678[Estimate])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Status"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A6:C10" totalsRowShown="0">
   <autoFilter ref="A6:C10"/>
   <tableColumns count="3">
@@ -1500,10 +1595,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H13">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
       <formula>"Accept"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1738,10 +1833,10 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H14">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
       <formula>"Accept"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2037,10 +2132,10 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:H15">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>"Accept"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2082,8 +2177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2284,6 +2379,291 @@
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G15">
         <f>SUM(Table1456[Estimate])</f>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="H3:H14">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+      <formula>"Accept"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F14">
+    <cfRule type="iconSet" priority="3">
+      <iconSet>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="#REF!"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H14">
+      <formula1>Status</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Information!$B$7:$B$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>F3:F14</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" customWidth="1"/>
+    <col min="4" max="4" width="47.42578125" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="2"/>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="2"/>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="2"/>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="2"/>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="2"/>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="2"/>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="2"/>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <f>SUM(Table14567[Estimate])</f>
         <v>4</v>
       </c>
     </row>
@@ -2333,12 +2713,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2355,7 +2735,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -2398,7 +2778,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D3" s="5"/>
       <c r="G3">
@@ -2410,7 +2790,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="2"/>
@@ -2423,7 +2803,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="2"/>
@@ -2433,7 +2813,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="2"/>
@@ -2443,7 +2823,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="2"/>
@@ -2452,21 +2832,13 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>85</v>
-      </c>
+      <c r="D8" s="6"/>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
-        <v>88</v>
-      </c>
       <c r="D9" s="6"/>
       <c r="E9" s="2"/>
     </row>
@@ -2508,7 +2880,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G15">
-        <f>SUM(Table14567[Estimate])</f>
+        <f>SUM(Table145678[Estimate])</f>
         <v>4</v>
       </c>
     </row>
@@ -2558,7 +2930,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:I19"/>
   <sheetViews>

</xml_diff>

<commit_message>
Map user story from product backlog to sprint backlog
</commit_message>
<xml_diff>
--- a/Document/SCRUM/Sprint Backlog.xlsx
+++ b/Document/SCRUM/Sprint Backlog.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="198">
   <si>
     <t>No.</t>
   </si>
@@ -1232,6 +1232,72 @@
   </si>
   <si>
     <t>Research</t>
+  </si>
+  <si>
+    <t>[Patient] View medical profile</t>
+  </si>
+  <si>
+    <t>[Patient] Update patient information</t>
+  </si>
+  <si>
+    <t>[Patient] Chat</t>
+  </si>
+  <si>
+    <t>[Patient] Show webcam</t>
+  </si>
+  <si>
+    <t>[Patient] Upload attachment</t>
+  </si>
+  <si>
+    <t>[Patient] View consult history</t>
+  </si>
+  <si>
+    <t>[Patient] Change profile picture</t>
+  </si>
+  <si>
+    <t>[Patient] Rating doctor</t>
+  </si>
+  <si>
+    <t>[Doctor] Create medical profile</t>
+  </si>
+  <si>
+    <t>[Doctor] Create patient</t>
+  </si>
+  <si>
+    <t>[Doctor] Add comment</t>
+  </si>
+  <si>
+    <t>[Doctor] Change picture profile</t>
+  </si>
+  <si>
+    <t>[Admin] Create doctor</t>
+  </si>
+  <si>
+    <t>[Admin] Define medical profile template</t>
+  </si>
+  <si>
+    <t>Report 3</t>
+  </si>
+  <si>
+    <t>Report 4</t>
+  </si>
+  <si>
+    <t>[Admin] Deactive/Active doctor</t>
+  </si>
+  <si>
+    <t>[Admin] Create patient</t>
+  </si>
+  <si>
+    <t>[User] Login</t>
+  </si>
+  <si>
+    <t>[Admin] View medical profile</t>
+  </si>
+  <si>
+    <t>[User] Forget password</t>
+  </si>
+  <si>
+    <t>[User] Register</t>
   </si>
 </sst>
 </file>
@@ -1334,6 +1400,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1343,8 +1411,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2387,8 +2453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2404,15 +2470,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
       <c r="H1" s="2" t="s">
         <v>54</v>
       </c>
@@ -2511,7 +2577,7 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="9" t="s">
         <v>174</v>
       </c>
       <c r="C6" t="s">
@@ -2534,7 +2600,7 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="8" t="s">
         <v>175</v>
       </c>
       <c r="C7" t="s">
@@ -2558,7 +2624,7 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="8" t="s">
         <v>175</v>
       </c>
       <c r="C8" t="s">
@@ -2582,7 +2648,7 @@
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="8" t="s">
         <v>175</v>
       </c>
       <c r="C9" t="s">
@@ -2744,7 +2810,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
     <col min="3" max="3" width="44.140625" customWidth="1"/>
     <col min="4" max="4" width="47.42578125" customWidth="1"/>
     <col min="5" max="5" width="29.85546875" customWidth="1"/>
@@ -2754,15 +2820,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
       <c r="H1" s="2" t="s">
         <v>162</v>
       </c>
@@ -2812,6 +2878,9 @@
       <c r="A4">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>194</v>
+      </c>
       <c r="C4" s="2" t="s">
         <v>136</v>
       </c>
@@ -2844,6 +2913,9 @@
       <c r="A6">
         <v>4</v>
       </c>
+      <c r="B6" s="9" t="s">
+        <v>183</v>
+      </c>
       <c r="C6" s="2" t="s">
         <v>138</v>
       </c>
@@ -2859,6 +2931,9 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>190</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>139</v>
@@ -2891,6 +2966,9 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>176</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>115</v>
@@ -3008,15 +3086,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
       <c r="H1" s="2" t="s">
         <v>163</v>
       </c>
@@ -3094,9 +3172,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>186</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>147</v>
@@ -3146,6 +3227,9 @@
       <c r="A9">
         <v>7</v>
       </c>
+      <c r="B9" s="9" t="s">
+        <v>187</v>
+      </c>
       <c r="C9" s="2" t="s">
         <v>150</v>
       </c>
@@ -3161,6 +3245,9 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>182</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>151</v>
@@ -3365,15 +3452,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
       <c r="H1" s="2" t="s">
         <v>167</v>
       </c>
@@ -3574,11 +3661,11 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
       <c r="H5" t="s">
         <v>21</v>
       </c>
@@ -3712,15 +3799,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
       <c r="H1" s="2" t="s">
         <v>109</v>
       </c>
@@ -3751,9 +3838,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>190</v>
       </c>
       <c r="C3" t="s">
         <v>56</v>
@@ -3772,6 +3862,9 @@
       <c r="A4">
         <v>2</v>
       </c>
+      <c r="B4" s="8" t="s">
+        <v>190</v>
+      </c>
       <c r="C4" t="s">
         <v>58</v>
       </c>
@@ -3789,9 +3882,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>191</v>
       </c>
       <c r="C5" t="s">
         <v>59</v>
@@ -3811,6 +3907,9 @@
       <c r="A6">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>191</v>
+      </c>
       <c r="C6" t="s">
         <v>61</v>
       </c>
@@ -3823,9 +3922,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>189</v>
       </c>
       <c r="C7" t="s">
         <v>60</v>
@@ -3945,15 +4047,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
       <c r="H1" s="2" t="s">
         <v>110</v>
       </c>
@@ -3984,10 +4086,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3" s="8" t="s">
+        <v>190</v>
+      </c>
       <c r="C3" t="s">
         <v>67</v>
       </c>
@@ -4001,9 +4106,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>191</v>
       </c>
       <c r="C4" t="s">
         <v>68</v>
@@ -4020,9 +4128,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>190</v>
       </c>
       <c r="C5" t="s">
         <v>69</v>
@@ -4036,9 +4147,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>190</v>
       </c>
       <c r="C6" t="s">
         <v>70</v>
@@ -4052,9 +4166,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>190</v>
       </c>
       <c r="C7" t="s">
         <v>71</v>
@@ -4068,9 +4185,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>190</v>
       </c>
       <c r="C8" t="s">
         <v>72</v>
@@ -4085,10 +4205,13 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
       <c r="B9" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="6" t="s">
         <v>73</v>
       </c>
       <c r="D9" s="4"/>
@@ -4100,9 +4223,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>192</v>
       </c>
       <c r="C10" t="s">
         <v>74</v>
@@ -4114,7 +4240,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
       </c>
       <c r="C11" t="s">
         <v>64</v>
@@ -4128,9 +4257,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>189</v>
       </c>
       <c r="C12" t="s">
         <v>65</v>
@@ -4145,7 +4277,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>191</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>66</v>
@@ -4160,7 +4295,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>190</v>
       </c>
       <c r="C14" t="s">
         <v>156</v>
@@ -4172,12 +4310,15 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E16" s="2"/>
     </row>
@@ -4237,15 +4378,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
       <c r="H1" s="2" t="s">
         <v>113</v>
       </c>
@@ -4280,6 +4421,9 @@
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>190</v>
+      </c>
       <c r="C3" t="s">
         <v>77</v>
       </c>
@@ -4298,6 +4442,9 @@
       <c r="A4">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>190</v>
+      </c>
       <c r="C4" t="s">
         <v>76</v>
       </c>
@@ -4316,6 +4463,9 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>191</v>
       </c>
       <c r="C5" t="s">
         <v>93</v>
@@ -4333,6 +4483,9 @@
       <c r="A6">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>190</v>
+      </c>
       <c r="C6" t="s">
         <v>75</v>
       </c>
@@ -4344,9 +4497,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>193</v>
       </c>
       <c r="C7" t="s">
         <v>78</v>
@@ -4362,9 +4518,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>188</v>
       </c>
       <c r="C8" t="s">
         <v>79</v>
@@ -4377,9 +4536,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>188</v>
       </c>
       <c r="C9" t="s">
         <v>82</v>
@@ -4399,6 +4561,9 @@
       <c r="A10">
         <v>8</v>
       </c>
+      <c r="B10" t="s">
+        <v>191</v>
+      </c>
       <c r="C10" t="s">
         <v>86</v>
       </c>
@@ -4414,6 +4579,9 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>190</v>
       </c>
       <c r="C11" t="s">
         <v>158</v>
@@ -4483,13 +4651,13 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.140625" customWidth="1"/>
     <col min="4" max="4" width="47.42578125" customWidth="1"/>
     <col min="5" max="5" width="29.85546875" customWidth="1"/>
@@ -4499,15 +4667,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
       <c r="H1" s="2" t="s">
         <v>112</v>
       </c>
@@ -4538,9 +4706,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>177</v>
       </c>
       <c r="C3" t="s">
         <v>87</v>
@@ -4560,6 +4731,9 @@
       <c r="A4">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>177</v>
+      </c>
       <c r="C4" t="s">
         <v>88</v>
       </c>
@@ -4575,9 +4749,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>178</v>
       </c>
       <c r="C5" t="s">
         <v>89</v>
@@ -4591,9 +4768,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>189</v>
       </c>
       <c r="C6" t="s">
         <v>90</v>
@@ -4611,6 +4791,9 @@
       <c r="A7">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>190</v>
+      </c>
       <c r="C7" t="s">
         <v>91</v>
       </c>
@@ -4623,9 +4806,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>188</v>
       </c>
       <c r="C8" t="s">
         <v>79</v>
@@ -4644,6 +4830,9 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="C9" t="s">
         <v>84</v>
@@ -4657,9 +4846,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>181</v>
       </c>
       <c r="C10" t="s">
         <v>98</v>
@@ -4767,15 +4959,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
       <c r="H1" s="2" t="s">
         <v>111</v>
       </c>
@@ -4806,9 +4998,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>178</v>
       </c>
       <c r="C3" t="s">
         <v>95</v>
@@ -4824,9 +5019,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>184</v>
       </c>
       <c r="C4" t="s">
         <v>96</v>
@@ -4843,19 +5041,25 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
+      <c r="B5" s="8" t="s">
+        <v>179</v>
+      </c>
       <c r="C5" t="s">
         <v>97</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>188</v>
       </c>
       <c r="C6" t="s">
         <v>79</v>
@@ -4869,9 +5073,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>178</v>
       </c>
       <c r="C7" t="s">
         <v>98</v>
@@ -4984,13 +5191,13 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.140625" customWidth="1"/>
     <col min="4" max="4" width="47.42578125" customWidth="1"/>
     <col min="5" max="5" width="29.85546875" customWidth="1"/>
@@ -5000,15 +5207,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
       <c r="H1" s="2" t="s">
         <v>114</v>
       </c>
@@ -5039,10 +5246,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3" s="8" t="s">
+        <v>189</v>
+      </c>
       <c r="C3" t="s">
         <v>101</v>
       </c>
@@ -5054,9 +5264,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>189</v>
       </c>
       <c r="C4" t="s">
         <v>102</v>
@@ -5070,9 +5283,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>189</v>
       </c>
       <c r="C5" t="s">
         <v>103</v>
@@ -5086,9 +5302,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>194</v>
       </c>
       <c r="C6" t="s">
         <v>104</v>
@@ -5102,9 +5321,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>176</v>
       </c>
       <c r="C7" t="s">
         <v>105</v>
@@ -5122,6 +5344,9 @@
       <c r="A8">
         <v>6</v>
       </c>
+      <c r="B8" t="s">
+        <v>176</v>
+      </c>
       <c r="C8" t="s">
         <v>106</v>
       </c>
@@ -5134,9 +5359,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>180</v>
       </c>
       <c r="C9" t="s">
         <v>107</v>
@@ -5150,9 +5378,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>179</v>
       </c>
       <c r="C10" t="s">
         <v>97</v>
@@ -5169,6 +5400,9 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>190</v>
       </c>
       <c r="C11" t="s">
         <v>108</v>
@@ -5244,13 +5478,13 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
     <col min="3" max="3" width="44.140625" customWidth="1"/>
     <col min="4" max="4" width="47.42578125" customWidth="1"/>
     <col min="5" max="5" width="29.85546875" customWidth="1"/>
@@ -5260,15 +5494,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
       <c r="H1" s="2" t="s">
         <v>160</v>
       </c>
@@ -5303,6 +5537,9 @@
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>176</v>
+      </c>
       <c r="C3" t="s">
         <v>115</v>
       </c>
@@ -5318,6 +5555,9 @@
       <c r="A4">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>190</v>
+      </c>
       <c r="C4" t="s">
         <v>108</v>
       </c>
@@ -5334,6 +5574,9 @@
       <c r="A5">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>191</v>
+      </c>
       <c r="C5" t="s">
         <v>116</v>
       </c>
@@ -5350,6 +5593,9 @@
       <c r="A6">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>190</v>
+      </c>
       <c r="C6" t="s">
         <v>117</v>
       </c>
@@ -5362,9 +5608,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>189</v>
       </c>
       <c r="C7" t="s">
         <v>118</v>
@@ -5378,9 +5627,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>179</v>
       </c>
       <c r="C8" t="s">
         <v>119</v>
@@ -5399,6 +5651,9 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>191</v>
       </c>
       <c r="C9" t="s">
         <v>121</v>
@@ -5506,7 +5761,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5522,15 +5777,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
       <c r="H1" s="2" t="s">
         <v>161</v>
       </c>
@@ -5565,6 +5820,9 @@
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3" s="9" t="s">
+        <v>183</v>
+      </c>
       <c r="C3" t="s">
         <v>127</v>
       </c>
@@ -5576,9 +5834,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>195</v>
       </c>
       <c r="C4" t="s">
         <v>128</v>
@@ -5592,9 +5853,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>196</v>
       </c>
       <c r="C5" t="s">
         <v>129</v>
@@ -5608,9 +5872,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>197</v>
       </c>
       <c r="C6" t="s">
         <v>130</v>
@@ -5627,6 +5894,9 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>190</v>
       </c>
       <c r="C7" t="s">
         <v>131</v>
@@ -5640,9 +5910,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>185</v>
       </c>
       <c r="C8" t="s">
         <v>132</v>
@@ -5658,9 +5931,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>176</v>
       </c>
       <c r="C9" t="s">
         <v>115</v>
@@ -5678,6 +5954,9 @@
       <c r="A10">
         <v>8</v>
       </c>
+      <c r="B10" t="s">
+        <v>133</v>
+      </c>
       <c r="C10" t="s">
         <v>133</v>
       </c>
@@ -5690,9 +5969,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>176</v>
       </c>
       <c r="C11" t="s">
         <v>134</v>

</xml_diff>